<commit_message>
Fix unassigned flight cost
</commit_message>
<xml_diff>
--- a/instances/instance1.xlsx
+++ b/instances/instance1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gstfrr/PycharmProjects/CrewSchedulingAndRecovery/instances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95E489D-E888-A54B-8596-CF511816DFDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F1E883-71BF-D441-B6E3-E482C05CA878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19500" activeTab="2" xr2:uid="{D8D3411D-76E6-224C-9079-3669CED563B0}"/>
   </bookViews>
@@ -792,7 +792,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -814,7 +814,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added docstrings and some type hints.
</commit_message>
<xml_diff>
--- a/instances/instance1.xlsx
+++ b/instances/instance1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gstfrr/PycharmProjects/CrewSchedulingAndRecovery/instances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F1E883-71BF-D441-B6E3-E482C05CA878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7020B9-8D06-AD48-8910-3072413E5333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19500" activeTab="2" xr2:uid="{D8D3411D-76E6-224C-9079-3669CED563B0}"/>
   </bookViews>
@@ -792,7 +792,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -822,7 +822,7 @@
         <v>27</v>
       </c>
       <c r="B3" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -830,7 +830,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -838,7 +838,7 @@
         <v>29</v>
       </c>
       <c r="B5" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Improve pairing generator, Flight constructor and other small details.
</commit_message>
<xml_diff>
--- a/instances/instance1.xlsx
+++ b/instances/instance1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gstfrr/PycharmProjects/CrewSchedulingAndRecovery/instances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7020B9-8D06-AD48-8910-3072413E5333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C300F0-131F-A148-A816-E1F77CA12EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19500" activeTab="2" xr2:uid="{D8D3411D-76E6-224C-9079-3669CED563B0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="21600" activeTab="1" xr2:uid="{D8D3411D-76E6-224C-9079-3669CED563B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Crew" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Flights!$A$1:$D$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Parameters!$A$1:$B$5</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
   <si>
     <t>John</t>
   </si>
@@ -110,15 +110,6 @@
     <t>LAX</t>
   </si>
   <si>
-    <t>ODR</t>
-  </si>
-  <si>
-    <t>VOV</t>
-  </si>
-  <si>
-    <t>WAR</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -138,12 +129,33 @@
   </si>
   <si>
     <t>INITIAL_DATE</t>
+  </si>
+  <si>
+    <t>ORD</t>
+  </si>
+  <si>
+    <t>MIA</t>
+  </si>
+  <si>
+    <t>ATL</t>
+  </si>
+  <si>
+    <t>SFO</t>
+  </si>
+  <si>
+    <t>SEA</t>
+  </si>
+  <si>
+    <t>BOS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="yyyy/mm/dd\ hh:mm"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -186,11 +198,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,18 +612,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98965418-D9AF-6440-9451-66AA9203570F}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="22.1640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="20.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -620,10 +635,10 @@
       <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -634,11 +649,11 @@
       <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2">
-        <v>45444.708333333336</v>
-      </c>
-      <c r="D2" s="2">
-        <v>45444.854166666664</v>
+      <c r="C2" s="4">
+        <v>45451.25</v>
+      </c>
+      <c r="D2" s="4">
+        <v>45451.375</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -648,137 +663,249 @@
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="2">
-        <v>45444.34375</v>
-      </c>
-      <c r="D3" s="2">
-        <v>45444.416666666664</v>
+      <c r="C3" s="4">
+        <v>45451.395833333336</v>
+      </c>
+      <c r="D3" s="4">
+        <v>45451.520833333336</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="2">
-        <v>45444.354166666664</v>
-      </c>
-      <c r="D4" s="2">
-        <v>45444.375</v>
+        <v>29</v>
+      </c>
+      <c r="C4" s="4">
+        <v>45451.541666666664</v>
+      </c>
+      <c r="D4" s="4">
+        <v>45451.708333333336</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="2">
-        <v>45444.458333333336</v>
-      </c>
-      <c r="D5" s="2">
-        <v>45444.541666666664</v>
+        <v>19</v>
+      </c>
+      <c r="C5" s="4">
+        <v>45451.729166666664</v>
+      </c>
+      <c r="D5" s="4">
+        <v>45451.833333333336</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="2">
-        <v>45444.458333333336</v>
-      </c>
-      <c r="D6" s="2">
-        <v>45444.708333333336</v>
+      <c r="C6" s="4">
+        <v>45452.25</v>
+      </c>
+      <c r="D6" s="4">
+        <v>45452.375</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="2">
-        <v>45444.25</v>
-      </c>
-      <c r="D7" s="2">
-        <v>45444.645833333336</v>
+        <v>20</v>
+      </c>
+      <c r="C7" s="4">
+        <v>45452.395833333336</v>
+      </c>
+      <c r="D7" s="4">
+        <v>45452.625</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="2">
-        <v>45444.458333333336</v>
-      </c>
-      <c r="D8" s="2">
-        <v>45444.614583333336</v>
+        <v>29</v>
+      </c>
+      <c r="C8" s="4">
+        <v>45452.645833333336</v>
+      </c>
+      <c r="D8" s="4">
+        <v>45452.75</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="2">
-        <v>45444.291666666664</v>
-      </c>
-      <c r="D9" s="2">
-        <v>45444.427083333336</v>
+        <v>21</v>
+      </c>
+      <c r="C9" s="4">
+        <v>45452.770833333336</v>
+      </c>
+      <c r="D9" s="4">
+        <v>45452.895833333336</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="2">
-        <v>45444.354166666664</v>
-      </c>
-      <c r="D10" s="2">
-        <v>45444.395833333336</v>
+        <v>19</v>
+      </c>
+      <c r="C10" s="4">
+        <v>45452.916666666664</v>
+      </c>
+      <c r="D10" s="4">
+        <v>45453.041666666664</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="2">
-        <v>45444.5625</v>
-      </c>
-      <c r="D11" s="2">
-        <v>45444.729166666664</v>
+        <v>30</v>
+      </c>
+      <c r="C11" s="4">
+        <v>45453.25</v>
+      </c>
+      <c r="D11" s="4">
+        <v>45453.354166666664</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="4">
+        <v>45453.375</v>
+      </c>
+      <c r="D12" s="4">
+        <v>45453.458333333336</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="4">
+        <v>45453.479166666664</v>
+      </c>
+      <c r="D13" s="4">
+        <v>45453.5625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="4">
+        <v>45453.583333333336</v>
+      </c>
+      <c r="D14" s="4">
+        <v>45453.708333333336</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="4">
+        <v>45453.729166666664</v>
+      </c>
+      <c r="D15" s="4">
+        <v>45453.770833333336</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="4">
+        <v>45453.791666666664</v>
+      </c>
+      <c r="D16" s="4">
+        <v>45453.895833333336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="4">
+        <v>45454.25</v>
+      </c>
+      <c r="D17" s="4">
+        <v>45454.458333333336</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="2">
-        <v>45444.708333333336</v>
-      </c>
-      <c r="D12" s="2">
-        <v>45444.854166666664</v>
+      <c r="C18" s="4">
+        <v>45454.479166666664</v>
+      </c>
+      <c r="D18" s="4">
+        <v>45454.5625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="4">
+        <v>45454.583333333336</v>
+      </c>
+      <c r="D19" s="4">
+        <v>45454.645833333336</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="4">
+        <v>45454.666666666664</v>
+      </c>
+      <c r="D20" s="4">
+        <v>45454.8125</v>
       </c>
     </row>
   </sheetData>
@@ -791,7 +918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7CAF5E1-B066-EA4F-A369-4FABFB7927C7}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -806,12 +933,12 @@
         <v>18</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3">
         <v>0.5</v>
@@ -819,7 +946,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3">
         <v>0.5</v>
@@ -827,7 +954,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3">
         <v>0.5</v>
@@ -835,7 +962,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3">
         <v>0.5</v>
@@ -843,7 +970,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3">
         <v>0.2</v>
@@ -851,7 +978,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2">
         <v>45444</v>

</xml_diff>